<commit_message>
Updated with current status
</commit_message>
<xml_diff>
--- a/Project2/MetodosEJB.xlsx
+++ b/Project2/MetodosEJB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="20115" windowHeight="8520"/>
+    <workbookView xWindow="240" yWindow="96" windowWidth="20112" windowHeight="8520"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="57">
   <si>
     <t>Pagina</t>
   </si>
@@ -60,9 +60,6 @@
     <t>addBankTellerUser(userID, bankteller)</t>
   </si>
   <si>
-    <t>adiciona e associa ao user</t>
-  </si>
-  <si>
     <t>user home</t>
   </si>
   <si>
@@ -72,9 +69,6 @@
     <t>unfollowCompaniesUser(userID, companyID)</t>
   </si>
   <si>
-    <t>getSubscribedCompanies(userID, companyID)</t>
-  </si>
-  <si>
     <t>List companies</t>
   </si>
   <si>
@@ -124,6 +118,80 @@
   </si>
   <si>
     <t>listUserByCompany(companyID)</t>
+  </si>
+  <si>
+    <t>Exists</t>
+  </si>
+  <si>
+    <t>IUserBean-&gt;getUser(Long id)</t>
+  </si>
+  <si>
+    <t>IUserBean-&gt;getUser(String name)</t>
+  </si>
+  <si>
+    <t>IUserBean-&gt;updateUser(User user) 
+Actualiza os dados mais tem os campos de password, subscribed companies, etc.</t>
+  </si>
+  <si>
+    <t>Test Pending</t>
+  </si>
+  <si>
+    <t>Isecurity-&gt;UpdateUserCredentials(Credentials credentials)</t>
+  </si>
+  <si>
+    <t>Assignee</t>
+  </si>
+  <si>
+    <t>Filipe</t>
+  </si>
+  <si>
+    <t>getBankTellerList(String filterPattern) and 
+getBankTellerNameList(String filterpattern)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temos getBankTeller(Long userId). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temos setBankTeller(Long userId, Long companyId)
+</t>
+  </si>
+  <si>
+    <t>adiciona e associa ao user. 
+setBankTeller(Long userId, BankTeller bankTeller)</t>
+  </si>
+  <si>
+    <t>See Comments</t>
+  </si>
+  <si>
+    <t>getSubscribedCompanies(userID)</t>
+  </si>
+  <si>
+    <t>ISecurity-&gt;CheckUser(Credentials credentials)</t>
+  </si>
+  <si>
+    <t>Temos ISecurity-&gt;RegisterUser(Credentials credentials).
+Não passamos dados do utilizador</t>
+  </si>
+  <si>
+    <t>getfollowedCompanyList(Long id)</t>
+  </si>
+  <si>
+    <t>unfollowCompany(Long userId, Long companyId)</t>
+  </si>
+  <si>
+    <t>followCompany(Long userId, Long companyId)</t>
+  </si>
+  <si>
+    <t>getCompany(Long companyId)</t>
+  </si>
+  <si>
+    <t>IAdmin-&gt;getUserList(int sortType, int ageThreshold)</t>
+  </si>
+  <si>
+    <t>IAdmin-&gt;getCompanyList(String filterPattern, int sortType);</t>
+  </si>
+  <si>
+    <t>getUserFollowCompanyList(Long companyId, int sortType, int ageThreshold);</t>
   </si>
 </sst>
 </file>
@@ -159,8 +227,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -176,13 +247,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D32" totalsRowShown="0">
-  <autoFilter ref="A1:D32"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E32" totalsRowShown="0">
+  <autoFilter ref="A1:E32"/>
+  <tableColumns count="5">
     <tableColumn id="1" name="Pagina"/>
     <tableColumn id="2" name="Metodos EJB"/>
     <tableColumn id="3" name="Status"/>
     <tableColumn id="4" name="Obesrvação"/>
+    <tableColumn id="5" name="Assignee"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -475,20 +547,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.109375" customWidth="1"/>
+    <col min="4" max="4" width="51.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -501,169 +574,292 @@
       <c r="D1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="C4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="C6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>13</v>
       </c>
-      <c r="D15" t="s">
+      <c r="C15" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="C21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
+    <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>17</v>
-      </c>
-      <c r="D22" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="C24" t="s">
+        <v>34</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
+    <row r="26" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="C26" t="s">
+        <v>46</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" t="s">
+        <v>34</v>
+      </c>
+      <c r="D28" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="29" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>31</v>
-      </c>
-      <c r="D28" t="s">
+      <c r="C29" t="s">
+        <v>34</v>
+      </c>
+      <c r="D29" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
+      <c r="C30" t="s">
+        <v>34</v>
+      </c>
+      <c r="D30" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>34</v>
+      </c>
+      <c r="D31" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>35</v>
+        <v>33</v>
+      </c>
+      <c r="C32" t="s">
+        <v>34</v>
+      </c>
+      <c r="D32" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -680,7 +876,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -692,7 +888,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated with latest status
</commit_message>
<xml_diff>
--- a/Project2/MetodosEJB.xlsx
+++ b/Project2/MetodosEJB.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="56">
   <si>
     <t>Pagina</t>
   </si>
@@ -131,9 +131,6 @@
   <si>
     <t>IUserBean-&gt;updateUser(User user) 
 Actualiza os dados mais tem os campos de password, subscribed companies, etc.</t>
-  </si>
-  <si>
-    <t>Test Pending</t>
   </si>
   <si>
     <t>Isecurity-&gt;UpdateUserCredentials(Credentials credentials)</t>
@@ -549,8 +546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -575,7 +572,7 @@
         <v>5</v>
       </c>
       <c r="E1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -591,7 +588,7 @@
         <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -626,7 +623,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>37</v>
@@ -642,13 +639,13 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" t="s">
         <v>38</v>
       </c>
-      <c r="D9" t="s">
-        <v>39</v>
-      </c>
       <c r="E9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -661,10 +658,10 @@
         <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -672,10 +669,10 @@
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -683,10 +680,10 @@
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -699,10 +696,10 @@
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -712,13 +709,13 @@
     </row>
     <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C17" t="s">
         <v>34</v>
       </c>
       <c r="D17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -729,7 +726,7 @@
         <v>34</v>
       </c>
       <c r="D18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -745,7 +742,7 @@
         <v>34</v>
       </c>
       <c r="D20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -756,7 +753,7 @@
         <v>34</v>
       </c>
       <c r="D21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -783,7 +780,7 @@
         <v>34</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -796,10 +793,10 @@
         <v>23</v>
       </c>
       <c r="C26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -826,7 +823,7 @@
         <v>34</v>
       </c>
       <c r="D29" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -837,7 +834,7 @@
         <v>34</v>
       </c>
       <c r="D30" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -848,7 +845,7 @@
         <v>34</v>
       </c>
       <c r="D31" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -859,7 +856,7 @@
         <v>34</v>
       </c>
       <c r="D32" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>